<commit_message>
updated till extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/RegistrationAsInstituteThroughOnborading.xlsx
+++ b/src/test/resources/testData/RegistrationAsInstituteThroughOnborading.xlsx
@@ -5,11 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="RegistrationData" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="RegistrationforInsitute" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="RegistrationforInsitute" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">FullName</t>
   </si>
@@ -65,13 +64,10 @@
     <t xml:space="preserve">Bidar</t>
   </si>
   <si>
-    <t xml:space="preserve">C:\Users\User\git\SNI-Framework\src\test\resources\testData\sample.jpg</t>
+    <t xml:space="preserve">C:\Users\User\git\SNI-Framework\src\test\resources\sample.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">welcome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\Users\User\git\SNI-Framework\src\test\resources\sample.jpg</t>
   </si>
 </sst>
 </file>
@@ -105,21 +101,15 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -127,13 +117,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -160,24 +143,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -204,104 +175,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="105.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16379" style="1" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>5689568956</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="sampleTestInstitute@gmail.com"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -315,7 +189,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -363,7 +237,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>15</v>

</xml_diff>